<commit_message>
use svg instead of png
</commit_message>
<xml_diff>
--- a/doseminimal-hl7conf.xlsx
+++ b/doseminimal-hl7conf.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\codes\fhir-radiation-dose-summary-ig\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A241D32A-A75F-40E3-9458-544E42E0ED3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EEFB48-A49D-416A-910E-560FDA28930E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F2D71892-AF68-403A-B289-9EDD46FACFF4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F2D71892-AF68-403A-B289-9EDD46FACFF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="67">
   <si>
     <t>Y</t>
   </si>
@@ -160,6 +161,81 @@
   </si>
   <si>
     <t>Dose (RP) Total</t>
+  </si>
+  <si>
+    <t>In order to go from excel to html you need to :</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Copy the excel cells to MS word</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>Save the MS word as html</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>Open the html in notepad++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. </t>
+  </si>
+  <si>
+    <t>Replace all \n by nothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. </t>
+  </si>
+  <si>
+    <t>Replace all \r by nothing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. </t>
+  </si>
+  <si>
+    <t>Use pretty XML formatting to format the table</t>
+  </si>
+  <si>
+    <t>Copy the table element in a new file</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>In table element, replace the style border-collapse: collapse by 'border-collapse: unset'</t>
+  </si>
+  <si>
+    <t>Make sure the cells are well displayed (readjust the with of cells if needed)</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>Replace 'background:#D9E1F2;' by 'background:#D9E1F2;vertical-align: middle;'</t>
+  </si>
+  <si>
+    <t>11.</t>
+  </si>
+  <si>
+    <t>Replace 'background:#C6E0B4;' by 'background:#C6E0B4;vertical-align: middle;'</t>
+  </si>
+  <si>
+    <t>12.</t>
+  </si>
+  <si>
+    <t>Remove from table element the style: margin-left:21.0pt;</t>
   </si>
 </sst>
 </file>
@@ -906,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD613B44-00F0-47B6-9F79-CDF6C9E7DD74}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1868,6 +1944,122 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5073A7C1-1820-4ADB-B1CC-3C57428FBE86}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1987,18 +2179,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2018,6 +2210,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FCF22D9-23E6-4F9D-8548-CAD3646BA1A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C9949E0-2D20-440F-94EC-C3E8372C7807}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2030,12 +2230,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FCF22D9-23E6-4F9D-8548-CAD3646BA1A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>